<commit_message>
Imported geographic location [GAZ:00000448]
</commit_message>
<xml_diff>
--- a/UpperLevel/GMHO_External_Imports.xlsx
+++ b/UpperLevel/GMHO_External_Imports.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -912,6 +912,28 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>GAZ</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>entity [BFO:0000001]</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>geographic location [GAZ:00000448]</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Imported material entity [BFO:0000040]
</commit_message>
<xml_diff>
--- a/UpperLevel/GMHO_External_Imports.xlsx
+++ b/UpperLevel/GMHO_External_Imports.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -934,6 +934,28 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>BFO</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>entity [BFO:0000001]</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>material entity [BFO:0000040]</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Imported planned process [COB:0000082]
</commit_message>
<xml_diff>
--- a/UpperLevel/GMHO_External_Imports.xlsx
+++ b/UpperLevel/GMHO_External_Imports.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -956,6 +956,28 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>COB</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>entity [BFO:0000001]</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>planned process [COB:0000082]</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Imported research study [SEPIO:0000125]
</commit_message>
<xml_diff>
--- a/UpperLevel/GMHO_External_Imports.xlsx
+++ b/UpperLevel/GMHO_External_Imports.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -978,6 +978,28 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SEPIO</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>entity [BFO:0000001]</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>research study [SEPIO:0000125]</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>